<commit_message>
fixed time: on client
</commit_message>
<xml_diff>
--- a/backend/processed_data.xlsx
+++ b/backend/processed_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnyRicmo\Documents\voting system\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFBBC0F-3005-40ED-A30B-7F4AD5AAA94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823180B7-525E-4BAA-ABB8-2E28CED96B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update data head from demo number to nss number
</commit_message>
<xml_diff>
--- a/backend/processed_data.xlsx
+++ b/backend/processed_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnyRicmo\Documents\voting system\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823180B7-525E-4BAA-ABB8-2E28CED96B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A8BC4C-3AB9-48E7-91D6-57EA800E77B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
-    <t>DEMO NUMBER</t>
-  </si>
-  <si>
     <t>DEMOPCO8492625</t>
   </si>
   <si>
@@ -83,6 +80,9 @@
   </si>
   <si>
     <t>DEMOPCO84926K</t>
+  </si>
+  <si>
+    <t>NSS NUMBER</t>
   </si>
 </sst>
 </file>
@@ -461,9 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -472,107 +470,107 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>